<commit_message>
fichier de finition de la première partie du stage stat_descriptive
</commit_message>
<xml_diff>
--- a/semaine 1 stage cahier des charges/données complètes_9 classes_MEFG_stagiaire statistique.xlsx
+++ b/semaine 1 stage cahier des charges/données complètes_9 classes_MEFG_stagiaire statistique.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golds\Documents\Thèse\04_étude observationnelle MEFG\03_données quantitatives MEFG\stagiaire statistique\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AEEC68-3983-484A-BDEB-A3FFF33E54B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={009B0092-0036-474C-9A45-0058008E000E}</author>
     <author>tc={00A500D4-00EB-405B-897E-00A4009F007F}</author>
@@ -83,418 +77,786 @@
     <author>tc={00B6006A-0021-41B7-A6A4-00F1001D0091}</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{009B0092-0036-474C-9A45-0058008E000E}">
+    <comment ref="C1" authorId="0">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Name of the subject
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{00A500D4-00EB-405B-897E-00A4009F007F}">
+    <comment ref="D1" authorId="1">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Filename of the subject
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00D80002-0042-4DFE-9CBB-00630096004F}">
+    <comment ref="E1" authorId="2">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Epoch length in seconds
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="3" shapeId="0" xr:uid="{00F60046-00BC-425F-93A2-003500B7009D}">
+    <comment ref="G1" authorId="3">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     The weight of the subject in kg
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="4" shapeId="0" xr:uid="{00540086-00A8-4855-B70D-008700C30005}">
+    <comment ref="H1" authorId="4">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     The age of the subject in years
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="5" shapeId="0" xr:uid="{006F00A1-0046-44E7-A3C8-00FD00710093}">
+    <comment ref="I1" authorId="5">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     The gender of the subject
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="6" shapeId="0" xr:uid="{0008006F-004A-4C90-AC66-007500120009}">
+    <comment ref="J1" authorId="6">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     kcals for this dataset
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="7" shapeId="0" xr:uid="{0045006F-001C-441E-BF02-00FE00260077}">
+    <comment ref="K1" authorId="7">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     (kcals / calendar days) for this dataset
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="8" shapeId="0" xr:uid="{00D900D4-007E-4C8C-A24A-005D001B00B9}">
+    <comment ref="L1" authorId="8">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     (kcals / whole hours) for this dataset
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="9" shapeId="0" xr:uid="{001500CC-0078-464C-947B-007A006A00EB}">
+    <comment ref="M1" authorId="9">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     MET rate for this dataset
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="10" shapeId="0" xr:uid="{002500C1-00E9-473A-9334-001100D500CB}">
+    <comment ref="N1" authorId="10">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of time in Sedentary in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="11" shapeId="0" xr:uid="{0028002F-00DA-4D23-9019-003800DC00D9}">
+    <comment ref="O1" authorId="11">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of time in Light in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="12" shapeId="0" xr:uid="{00EB00D8-0065-4A0B-80F2-006500AF0027}">
+    <comment ref="P1" authorId="12">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of time in Moderate in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="13" shapeId="0" xr:uid="{00790020-0091-4108-ADD0-002200BE0088}">
+    <comment ref="Q1" authorId="13">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of time in Vigorous in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="14" shapeId="0" xr:uid="{00CB0021-0071-4950-B840-004E004100C9}">
+    <comment ref="R1" authorId="14">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Percentage of time in Sedentary
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="15" shapeId="0" xr:uid="{000C00FF-005C-4DA4-86EF-00900030005A}">
+    <comment ref="S1" authorId="15">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Percentage of time in Light
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="16" shapeId="0" xr:uid="{00FA00A5-0056-41D7-8FE8-00D700DB007B}">
+    <comment ref="T1" authorId="16">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Percentage of time in Moderate
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="17" shapeId="0" xr:uid="{002A0004-00BB-4169-BFF0-00DD008E0097}">
+    <comment ref="U1" authorId="17">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Percentage of time in Vigorous
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="18" shapeId="0" xr:uid="{005500D4-003E-498A-AF34-00CE006D0070}">
+    <comment ref="V1" authorId="18">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of time in MVPA in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="19" shapeId="0" xr:uid="{006F004F-008C-49AF-832B-008600840068}">
+    <comment ref="W1" authorId="19">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Percent of time spent in MVPA
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="20" shapeId="0" xr:uid="{00B20069-00C8-4F14-BE11-0098003A001E}">
+    <comment ref="X1" authorId="20">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average amount of MVPA per calendar day in minutes
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="21" shapeId="0" xr:uid="{001F007E-00FC-460B-AF16-00B8006C005C}">
+    <comment ref="Y1" authorId="21">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Sum of counts for Axis 1 (Y-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="22" shapeId="0" xr:uid="{00C90005-002B-411D-983A-00B800F400E0}">
+    <comment ref="Z1" authorId="22">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Sum of counts for Axis 2 (X-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="23" shapeId="0" xr:uid="{004000DE-00DB-472D-972E-000700EF00FF}">
+    <comment ref="AA1" authorId="23">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Sum of counts for Axis 3 (Z-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="24" shapeId="0" xr:uid="{00210072-00ED-42CE-A9BF-002C00E50013}">
+    <comment ref="AB1" authorId="24">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average of counts for Axis 1 (Y-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="25" shapeId="0" xr:uid="{00A500DD-00BE-41DF-AFB1-00BA0023004A}">
+    <comment ref="AC1" authorId="25">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average of counts for Axis 2 (X-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="26" shapeId="0" xr:uid="{006C00B5-00EE-4AB3-A2FD-0022003B0053}">
+    <comment ref="AD1" authorId="26">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average of counts for Axis 3 (Z-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="27" shapeId="0" xr:uid="{003500E9-005E-4374-A11D-008500260014}">
+    <comment ref="AE1" authorId="27">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum count value for Axis 1 (Y-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="28" shapeId="0" xr:uid="{00810043-009E-40A1-964E-00A000C600E2}">
+    <comment ref="AF1" authorId="28">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum count value for Axis 2 (X-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="29" shapeId="0" xr:uid="{00CF00FE-00E1-4512-8F8C-0092008600E0}">
+    <comment ref="AG1" authorId="29">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum count value for Axis 3 (Z-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="30" shapeId="0" xr:uid="{00C20072-0029-4D63-B1F8-000B008200C1}">
+    <comment ref="AH1" authorId="30">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Counts Per Minute for Axis 1 (Y-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="31" shapeId="0" xr:uid="{004300CB-0074-4A62-A6C7-008A00040022}">
+    <comment ref="AI1" authorId="31">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Counts Per Minute for Axis 2 (X-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="32" shapeId="0" xr:uid="{002F00FE-00DB-4632-9418-00C9005200E4}">
+    <comment ref="AJ1" authorId="32">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Counts Per Minute for Axis 3 (Z-Axis)
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="33" shapeId="0" xr:uid="{002D0064-007F-4E24-B7C3-00220082005F}">
+    <comment ref="AK1" authorId="33">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Vector Magnitude of all 3 Axis
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="34" shapeId="0" xr:uid="{00F800FD-0090-4814-9A51-002C009500AB}">
+    <comment ref="AL1" authorId="34">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average Vector Magnitude of all 3 Axis
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="35" shapeId="0" xr:uid="{002300DF-0068-4190-B3E0-00B8009100C6}">
+    <comment ref="AM1" authorId="35">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum Vector Magnitude of all 3 Axis
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="36" shapeId="0" xr:uid="{008C0049-0076-4D82-B95A-00C100940029}">
+    <comment ref="AN1" authorId="36">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Vector Magnitude Counts Per Minute
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="37" shapeId="0" xr:uid="{00EF001E-00E1-47C2-B118-00A900730026}">
+    <comment ref="AO1" authorId="37">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Sum of Step Counts
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="38" shapeId="0" xr:uid="{00FA005C-00A2-4B0B-90F3-0064007E002C}">
+    <comment ref="AP1" authorId="38">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average Step Counts
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="39" shapeId="0" xr:uid="{002100B0-00FF-4CF8-BD5B-008D000A00C0}">
+    <comment ref="AQ1" authorId="39">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum Step Counts
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="40" shapeId="0" xr:uid="{00D4006A-00E2-4025-9C3F-0077000400FD}">
+    <comment ref="AR1" authorId="40">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Steps Per Minute
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="41" shapeId="0" xr:uid="{00910038-004F-4466-A9A1-0009004400AF}">
+    <comment ref="AS1" authorId="41">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Average Lux Value
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AT1" authorId="42" shapeId="0" xr:uid="{007E00D9-004D-4657-92FB-00E3007500DF}">
+    <comment ref="AT1" authorId="42">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Maximum Lux Value
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AU1" authorId="43" shapeId="0" xr:uid="{00A400CC-0096-49C1-A86B-0099003100C0}">
+    <comment ref="AU1" authorId="43">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Number of epochs
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AV1" authorId="44" shapeId="0" xr:uid="{00550012-00DF-45C4-BEAD-00EE00650008}">
+    <comment ref="AV1" authorId="44">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Length of scored time
 </t>
+        </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="45" shapeId="0" xr:uid="{00B6006A-0021-41B7-A6A4-00F1001D0091}">
+    <comment ref="AW1" authorId="45">
       <text>
-        <t xml:space="preserve">[Commentaire à thread]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
 Commentaire :
     Number of Calendar Days
 </t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -3684,11 +4046,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4449,14 +4811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV11" sqref="AV11"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="11.5546875" style="8"/>
     <col min="3" max="3" width="25.88671875" style="8" customWidth="1"/>
@@ -4473,7 +4835,7 @@
     <col min="56" max="16384" width="11.5546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" s="6" customFormat="1">
       <c r="A1" s="42" t="s">
         <v>1058</v>
       </c>
@@ -4640,7 +5002,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="2" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" s="31" customFormat="1">
       <c r="A2" s="28" t="s">
         <v>46</v>
       </c>
@@ -4807,7 +5169,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="3" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" s="31" customFormat="1">
       <c r="A3" s="28" t="s">
         <v>46</v>
       </c>
@@ -4974,7 +5336,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" s="31" customFormat="1">
       <c r="A4" s="28" t="s">
         <v>46</v>
       </c>
@@ -5141,7 +5503,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="5" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A5" s="28" t="s">
         <v>46</v>
       </c>
@@ -5308,7 +5670,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="6" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" s="31" customFormat="1">
       <c r="A6" s="28" t="s">
         <v>46</v>
       </c>
@@ -5475,7 +5837,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="7" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" s="31" customFormat="1">
       <c r="A7" s="28" t="s">
         <v>46</v>
       </c>
@@ -5642,7 +6004,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="8" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" s="31" customFormat="1">
       <c r="A8" s="28" t="s">
         <v>46</v>
       </c>
@@ -5807,7 +6169,7 @@
       </c>
       <c r="BC8" s="34"/>
     </row>
-    <row r="9" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" s="31" customFormat="1">
       <c r="A9" s="28" t="s">
         <v>46</v>
       </c>
@@ -5974,7 +6336,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="10" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" s="31" customFormat="1">
       <c r="A10" s="28" t="s">
         <v>46</v>
       </c>
@@ -6141,7 +6503,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A11" s="28" t="s">
         <v>46</v>
       </c>
@@ -6306,7 +6668,7 @@
       </c>
       <c r="BC11" s="34"/>
     </row>
-    <row r="12" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A12" s="28" t="s">
         <v>46</v>
       </c>
@@ -6471,7 +6833,7 @@
       </c>
       <c r="BC12" s="34"/>
     </row>
-    <row r="13" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" s="31" customFormat="1">
       <c r="A13" s="28" t="s">
         <v>46</v>
       </c>
@@ -6638,7 +7000,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="14" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" s="31" customFormat="1">
       <c r="A14" s="28" t="s">
         <v>46</v>
       </c>
@@ -6805,7 +7167,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="15" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" ht="28.8">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -6972,7 +7334,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -7139,7 +7501,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" ht="28.8">
       <c r="A17" s="7" t="s">
         <v>46</v>
       </c>
@@ -7304,7 +7666,7 @@
       </c>
       <c r="BC17" s="22"/>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -7471,7 +7833,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="19" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" ht="28.8">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -7638,7 +8000,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55">
       <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
@@ -7805,7 +8167,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
@@ -7972,7 +8334,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="22" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" ht="28.8">
       <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
@@ -8139,7 +8501,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55">
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
@@ -8306,7 +8668,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55">
       <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
@@ -8473,7 +8835,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55">
       <c r="A25" s="7" t="s">
         <v>46</v>
       </c>
@@ -8640,7 +9002,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="26" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" ht="28.8">
       <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
@@ -8807,7 +9169,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="27" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" ht="28.8">
       <c r="A27" s="7" t="s">
         <v>46</v>
       </c>
@@ -8974,7 +9336,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:55">
       <c r="A28" s="7" t="s">
         <v>46</v>
       </c>
@@ -9141,7 +9503,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:55">
       <c r="A29" s="7" t="s">
         <v>46</v>
       </c>
@@ -9306,7 +9668,7 @@
       </c>
       <c r="BC29" s="22"/>
     </row>
-    <row r="30" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:55" ht="28.8">
       <c r="A30" s="7" t="s">
         <v>46</v>
       </c>
@@ -9473,7 +9835,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="31" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:55" s="31" customFormat="1">
       <c r="A31" s="28" t="s">
         <v>205</v>
       </c>
@@ -9640,7 +10002,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="32" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:55" s="31" customFormat="1">
       <c r="A32" s="28" t="s">
         <v>205</v>
       </c>
@@ -9805,7 +10167,7 @@
       </c>
       <c r="BC32" s="37"/>
     </row>
-    <row r="33" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:55" s="31" customFormat="1">
       <c r="A33" s="28" t="s">
         <v>205</v>
       </c>
@@ -9972,7 +10334,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="34" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A34" s="28" t="s">
         <v>205</v>
       </c>
@@ -10139,7 +10501,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="35" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A35" s="28" t="s">
         <v>205</v>
       </c>
@@ -10306,7 +10668,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="36" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:55" s="31" customFormat="1">
       <c r="A36" s="28" t="s">
         <v>205</v>
       </c>
@@ -10473,7 +10835,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="37" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A37" s="28" t="s">
         <v>205</v>
       </c>
@@ -10640,7 +11002,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="38" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:55" s="31" customFormat="1">
       <c r="A38" s="28" t="s">
         <v>205</v>
       </c>
@@ -10807,7 +11169,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="39" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A39" s="28" t="s">
         <v>205</v>
       </c>
@@ -10974,7 +11336,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="40" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A40" s="28" t="s">
         <v>205</v>
       </c>
@@ -11141,7 +11503,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="41" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:55" s="31" customFormat="1">
       <c r="A41" s="28" t="s">
         <v>205</v>
       </c>
@@ -11308,7 +11670,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="42" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:55" s="31" customFormat="1">
       <c r="A42" s="28" t="s">
         <v>205</v>
       </c>
@@ -11475,7 +11837,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="43" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A43" s="28" t="s">
         <v>205</v>
       </c>
@@ -11642,7 +12004,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="44" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A44" s="28" t="s">
         <v>205</v>
       </c>
@@ -11809,7 +12171,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="45" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:55" s="31" customFormat="1">
       <c r="A45" s="28" t="s">
         <v>205</v>
       </c>
@@ -11976,7 +12338,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="46" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:55" s="31" customFormat="1">
       <c r="A46" s="38" t="s">
         <v>1005</v>
       </c>
@@ -12143,7 +12505,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="47" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:55" s="31" customFormat="1">
       <c r="A47" s="28" t="s">
         <v>205</v>
       </c>
@@ -12310,7 +12672,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="48" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A48" s="28" t="s">
         <v>205</v>
       </c>
@@ -12477,7 +12839,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="49" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:55" s="31" customFormat="1">
       <c r="A49" s="28" t="s">
         <v>205</v>
       </c>
@@ -12644,7 +13006,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A50" s="28" t="s">
         <v>205</v>
       </c>
@@ -12811,7 +13173,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="51" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A51" s="28" t="s">
         <v>205</v>
       </c>
@@ -12978,7 +13340,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="52" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:55" ht="28.8">
       <c r="A52" s="7" t="s">
         <v>205</v>
       </c>
@@ -13145,7 +13507,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="53" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:55" ht="28.8">
       <c r="A53" s="7" t="s">
         <v>205</v>
       </c>
@@ -13312,7 +13674,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:55">
       <c r="A54" s="7" t="s">
         <v>205</v>
       </c>
@@ -13479,7 +13841,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:55">
       <c r="A55" s="7" t="s">
         <v>205</v>
       </c>
@@ -13646,7 +14008,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="56" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:55" ht="28.8">
       <c r="A56" s="7" t="s">
         <v>205</v>
       </c>
@@ -13813,7 +14175,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:55">
       <c r="A57" s="7" t="s">
         <v>205</v>
       </c>
@@ -13980,7 +14342,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:55">
       <c r="A58" s="7" t="s">
         <v>205</v>
       </c>
@@ -14147,7 +14509,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="59" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:55" ht="28.8">
       <c r="A59" s="7" t="s">
         <v>205</v>
       </c>
@@ -14314,7 +14676,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="60" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:55" ht="28.8">
       <c r="A60" s="7" t="s">
         <v>205</v>
       </c>
@@ -14481,7 +14843,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:55">
       <c r="A61" s="7" t="s">
         <v>205</v>
       </c>
@@ -14648,7 +15010,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="62" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:55">
       <c r="A62" s="7" t="s">
         <v>205</v>
       </c>
@@ -14815,7 +15177,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="63" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:55" ht="28.8">
       <c r="A63" s="7" t="s">
         <v>205</v>
       </c>
@@ -14982,7 +15344,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="64" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:55" ht="28.8">
       <c r="A64" s="7" t="s">
         <v>205</v>
       </c>
@@ -15149,7 +15511,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:55">
       <c r="A65" s="7" t="s">
         <v>205</v>
       </c>
@@ -15316,7 +15678,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="66" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:55">
       <c r="A66" s="7" t="s">
         <v>205</v>
       </c>
@@ -15483,7 +15845,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="67" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A67" s="28" t="s">
         <v>395</v>
       </c>
@@ -15650,7 +16012,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="68" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A68" s="28" t="s">
         <v>395</v>
       </c>
@@ -15817,7 +16179,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="69" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:55" s="31" customFormat="1">
       <c r="A69" s="28" t="s">
         <v>395</v>
       </c>
@@ -15980,7 +16342,7 @@
       <c r="BB69" s="37"/>
       <c r="BC69" s="37"/>
     </row>
-    <row r="70" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:55" s="31" customFormat="1">
       <c r="A70" s="28" t="s">
         <v>395</v>
       </c>
@@ -16143,7 +16505,7 @@
       <c r="BB70" s="37"/>
       <c r="BC70" s="37"/>
     </row>
-    <row r="71" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A71" s="28" t="s">
         <v>395</v>
       </c>
@@ -16310,7 +16672,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="72" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:55" s="31" customFormat="1">
       <c r="A72" s="28" t="s">
         <v>395</v>
       </c>
@@ -16477,7 +16839,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="73" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:55" s="31" customFormat="1">
       <c r="A73" s="28" t="s">
         <v>395</v>
       </c>
@@ -16640,7 +17002,7 @@
       <c r="BB73" s="37"/>
       <c r="BC73" s="37"/>
     </row>
-    <row r="74" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:55" s="31" customFormat="1">
       <c r="A74" s="28" t="s">
         <v>395</v>
       </c>
@@ -16807,7 +17169,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="75" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A75" s="28" t="s">
         <v>395</v>
       </c>
@@ -16972,7 +17334,7 @@
       </c>
       <c r="BC75" s="37"/>
     </row>
-    <row r="76" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:55" s="31" customFormat="1">
       <c r="A76" s="28" t="s">
         <v>395</v>
       </c>
@@ -17139,7 +17501,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="77" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A77" s="28" t="s">
         <v>395</v>
       </c>
@@ -17306,7 +17668,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="78" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:55" s="31" customFormat="1">
       <c r="A78" s="28" t="s">
         <v>395</v>
       </c>
@@ -17473,7 +17835,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="79" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A79" s="28" t="s">
         <v>395</v>
       </c>
@@ -17640,7 +18002,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="80" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:55" s="31" customFormat="1">
       <c r="A80" s="28" t="s">
         <v>395</v>
       </c>
@@ -17807,7 +18169,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="81" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A81" s="28" t="s">
         <v>395</v>
       </c>
@@ -17974,7 +18336,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="82" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A82" s="28" t="s">
         <v>395</v>
       </c>
@@ -18141,7 +18503,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="83" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:55" s="31" customFormat="1">
       <c r="A83" s="28" t="s">
         <v>395</v>
       </c>
@@ -18306,7 +18668,7 @@
       </c>
       <c r="BC83" s="37"/>
     </row>
-    <row r="84" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:55" s="31" customFormat="1">
       <c r="A84" s="28" t="s">
         <v>395</v>
       </c>
@@ -18473,7 +18835,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="85" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:55" s="31" customFormat="1">
       <c r="A85" s="28" t="s">
         <v>395</v>
       </c>
@@ -18640,7 +19002,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="86" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:55" s="31" customFormat="1">
       <c r="A86" s="28" t="s">
         <v>395</v>
       </c>
@@ -18807,7 +19169,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="87" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A87" s="28" t="s">
         <v>395</v>
       </c>
@@ -18972,7 +19334,7 @@
       </c>
       <c r="BC87" s="37"/>
     </row>
-    <row r="88" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:55">
       <c r="A88" s="7" t="s">
         <v>395</v>
       </c>
@@ -19139,7 +19501,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="89" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:55" ht="28.8">
       <c r="A89" s="7" t="s">
         <v>395</v>
       </c>
@@ -19304,7 +19666,7 @@
       </c>
       <c r="BC89" s="22"/>
     </row>
-    <row r="90" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:55" ht="28.8">
       <c r="A90" s="7" t="s">
         <v>395</v>
       </c>
@@ -19471,7 +19833,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="91" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:55">
       <c r="A91" s="7" t="s">
         <v>395</v>
       </c>
@@ -19638,7 +20000,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="92" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:55">
       <c r="A92" s="7" t="s">
         <v>395</v>
       </c>
@@ -19805,7 +20167,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="93" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:55" ht="28.8">
       <c r="A93" s="7" t="s">
         <v>395</v>
       </c>
@@ -19972,7 +20334,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="94" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:55" ht="28.8">
       <c r="A94" s="7" t="s">
         <v>395</v>
       </c>
@@ -20139,7 +20501,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="95" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:55">
       <c r="A95" s="7" t="s">
         <v>395</v>
       </c>
@@ -20302,7 +20664,7 @@
       <c r="BB95" s="22"/>
       <c r="BC95" s="22"/>
     </row>
-    <row r="96" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:55">
       <c r="A96" s="7" t="s">
         <v>395</v>
       </c>
@@ -20469,7 +20831,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="97" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:55" ht="28.8">
       <c r="A97" s="7" t="s">
         <v>395</v>
       </c>
@@ -20636,7 +20998,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="98" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:55">
       <c r="A98" s="7" t="s">
         <v>395</v>
       </c>
@@ -20801,7 +21163,7 @@
       </c>
       <c r="BC98" s="22"/>
     </row>
-    <row r="99" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:55">
       <c r="A99" s="7" t="s">
         <v>395</v>
       </c>
@@ -20968,7 +21330,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="100" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:55">
       <c r="A100" s="7" t="s">
         <v>395</v>
       </c>
@@ -21131,7 +21493,7 @@
       <c r="BB100" s="22"/>
       <c r="BC100" s="22"/>
     </row>
-    <row r="101" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:55">
       <c r="A101" s="7" t="s">
         <v>395</v>
       </c>
@@ -21298,7 +21660,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="102" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:55">
       <c r="A102" s="7" t="s">
         <v>395</v>
       </c>
@@ -21461,7 +21823,7 @@
       <c r="BB102" s="22"/>
       <c r="BC102" s="22"/>
     </row>
-    <row r="103" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:55">
       <c r="A103" s="7" t="s">
         <v>395</v>
       </c>
@@ -21628,7 +21990,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="104" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:55" ht="28.8">
       <c r="A104" s="7" t="s">
         <v>395</v>
       </c>
@@ -21795,7 +22157,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="105" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:55">
       <c r="A105" s="7" t="s">
         <v>395</v>
       </c>
@@ -21960,7 +22322,7 @@
       </c>
       <c r="BC105" s="22"/>
     </row>
-    <row r="106" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:55" ht="28.8">
       <c r="A106" s="7" t="s">
         <v>395</v>
       </c>
@@ -22127,7 +22489,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="107" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:55">
       <c r="A107" s="7" t="s">
         <v>395</v>
       </c>
@@ -22294,7 +22656,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="108" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:55">
       <c r="A108" s="7" t="s">
         <v>395</v>
       </c>
@@ -22461,7 +22823,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="109" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:55" s="31" customFormat="1">
       <c r="A109" s="28" t="s">
         <v>595</v>
       </c>
@@ -22628,7 +22990,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="110" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A110" s="28" t="s">
         <v>595</v>
       </c>
@@ -22795,7 +23157,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="111" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:55" s="31" customFormat="1">
       <c r="A111" s="28" t="s">
         <v>595</v>
       </c>
@@ -22962,7 +23324,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="112" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A112" s="28" t="s">
         <v>595</v>
       </c>
@@ -23129,7 +23491,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="113" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:55" s="31" customFormat="1">
       <c r="A113" s="28" t="s">
         <v>595</v>
       </c>
@@ -23294,7 +23656,7 @@
       </c>
       <c r="BC113" s="40"/>
     </row>
-    <row r="114" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:55" s="31" customFormat="1">
       <c r="A114" s="28" t="s">
         <v>595</v>
       </c>
@@ -23459,7 +23821,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="115" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:55" s="31" customFormat="1">
       <c r="A115" s="28" t="s">
         <v>595</v>
       </c>
@@ -23624,7 +23986,7 @@
       </c>
       <c r="BC115" s="40"/>
     </row>
-    <row r="116" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:55" s="31" customFormat="1">
       <c r="A116" s="28" t="s">
         <v>595</v>
       </c>
@@ -23789,7 +24151,7 @@
       </c>
       <c r="BC116" s="40"/>
     </row>
-    <row r="117" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:55" s="31" customFormat="1">
       <c r="A117" s="28" t="s">
         <v>595</v>
       </c>
@@ -23956,7 +24318,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="118" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:55" s="31" customFormat="1">
       <c r="A118" s="28" t="s">
         <v>595</v>
       </c>
@@ -24123,7 +24485,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="119" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:55" s="31" customFormat="1">
       <c r="A119" s="28" t="s">
         <v>595</v>
       </c>
@@ -24290,7 +24652,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="120" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:55" s="31" customFormat="1">
       <c r="A120" s="28" t="s">
         <v>595</v>
       </c>
@@ -24455,7 +24817,7 @@
       </c>
       <c r="BC120" s="40"/>
     </row>
-    <row r="121" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:55" s="31" customFormat="1">
       <c r="A121" s="28" t="s">
         <v>595</v>
       </c>
@@ -24622,7 +24984,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="122" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:55" s="31" customFormat="1">
       <c r="A122" s="28" t="s">
         <v>595</v>
       </c>
@@ -24789,7 +25151,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="123" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:55" s="31" customFormat="1">
       <c r="A123" s="28" t="s">
         <v>595</v>
       </c>
@@ -24956,7 +25318,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="124" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:55" s="31" customFormat="1">
       <c r="A124" s="28" t="s">
         <v>595</v>
       </c>
@@ -25123,7 +25485,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="125" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:55" s="31" customFormat="1">
       <c r="A125" s="28" t="s">
         <v>595</v>
       </c>
@@ -25290,7 +25652,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="126" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A126" s="28" t="s">
         <v>595</v>
       </c>
@@ -25457,7 +25819,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="127" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:55" ht="28.8">
       <c r="A127" s="7" t="s">
         <v>682</v>
       </c>
@@ -25624,7 +25986,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="128" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:55" ht="28.8">
       <c r="A128" s="7" t="s">
         <v>682</v>
       </c>
@@ -25791,7 +26153,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="129" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:55">
       <c r="A129" s="7" t="s">
         <v>682</v>
       </c>
@@ -25958,7 +26320,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="130" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:55">
       <c r="A130" s="7" t="s">
         <v>682</v>
       </c>
@@ -26125,7 +26487,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="131" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:55">
       <c r="A131" s="7" t="s">
         <v>682</v>
       </c>
@@ -26290,7 +26652,7 @@
       </c>
       <c r="BC131" s="22"/>
     </row>
-    <row r="132" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:55">
       <c r="A132" s="7" t="s">
         <v>682</v>
       </c>
@@ -26457,7 +26819,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="133" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:55">
       <c r="A133" s="7" t="s">
         <v>682</v>
       </c>
@@ -26624,7 +26986,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="134" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:55">
       <c r="A134" s="7" t="s">
         <v>682</v>
       </c>
@@ -26787,7 +27149,7 @@
       <c r="BB134" s="21"/>
       <c r="BC134" s="22"/>
     </row>
-    <row r="135" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:55" ht="28.8">
       <c r="A135" s="7" t="s">
         <v>682</v>
       </c>
@@ -26954,7 +27316,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="136" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:55">
       <c r="A136" s="7" t="s">
         <v>682</v>
       </c>
@@ -27121,7 +27483,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="137" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:55">
       <c r="A137" s="7" t="s">
         <v>682</v>
       </c>
@@ -27288,7 +27650,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="138" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:55" ht="28.8">
       <c r="A138" s="7" t="s">
         <v>682</v>
       </c>
@@ -27455,7 +27817,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="139" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:55">
       <c r="A139" s="7" t="s">
         <v>682</v>
       </c>
@@ -27622,7 +27984,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="140" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:55">
       <c r="A140" s="7" t="s">
         <v>682</v>
       </c>
@@ -27789,7 +28151,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="141" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:55">
       <c r="A141" s="7" t="s">
         <v>682</v>
       </c>
@@ -27954,7 +28316,7 @@
       </c>
       <c r="BC141" s="22"/>
     </row>
-    <row r="142" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:55" ht="28.8">
       <c r="A142" s="7" t="s">
         <v>682</v>
       </c>
@@ -28121,7 +28483,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="143" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:55">
       <c r="A143" s="7" t="s">
         <v>682</v>
       </c>
@@ -28288,7 +28650,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="144" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:55">
       <c r="A144" s="7" t="s">
         <v>682</v>
       </c>
@@ -28453,7 +28815,7 @@
       </c>
       <c r="BC144" s="22"/>
     </row>
-    <row r="145" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:55">
       <c r="A145" s="7" t="s">
         <v>682</v>
       </c>
@@ -28620,7 +28982,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="146" spans="1:55" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:55" ht="28.8">
       <c r="A146" s="7" t="s">
         <v>682</v>
       </c>
@@ -28787,7 +29149,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="147" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:55" s="31" customFormat="1">
       <c r="A147" s="28" t="s">
         <v>682</v>
       </c>
@@ -28954,7 +29316,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="148" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A148" s="28" t="s">
         <v>682</v>
       </c>
@@ -29121,7 +29483,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="149" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A149" s="28" t="s">
         <v>682</v>
       </c>
@@ -29288,7 +29650,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="150" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:55" s="31" customFormat="1">
       <c r="A150" s="28" t="s">
         <v>682</v>
       </c>
@@ -29455,7 +29817,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="151" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A151" s="28" t="s">
         <v>682</v>
       </c>
@@ -29622,7 +29984,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="152" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:55" s="31" customFormat="1">
       <c r="A152" s="28" t="s">
         <v>682</v>
       </c>
@@ -29785,7 +30147,7 @@
       <c r="BB152" s="37"/>
       <c r="BC152" s="37"/>
     </row>
-    <row r="153" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A153" s="28" t="s">
         <v>682</v>
       </c>
@@ -29952,7 +30314,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="154" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:55" s="31" customFormat="1">
       <c r="A154" s="28" t="s">
         <v>682</v>
       </c>
@@ -30119,7 +30481,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="155" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:55" s="31" customFormat="1">
       <c r="A155" s="28" t="s">
         <v>682</v>
       </c>
@@ -30280,7 +30642,7 @@
       <c r="BB155" s="37"/>
       <c r="BC155" s="37"/>
     </row>
-    <row r="156" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:55" s="31" customFormat="1">
       <c r="A156" s="28" t="s">
         <v>682</v>
       </c>
@@ -30445,7 +30807,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="157" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:55" s="31" customFormat="1">
       <c r="A157" s="28" t="s">
         <v>682</v>
       </c>
@@ -30612,7 +30974,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="158" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:55" s="31" customFormat="1">
       <c r="A158" s="28" t="s">
         <v>682</v>
       </c>
@@ -30775,7 +31137,7 @@
       <c r="BB158" s="37"/>
       <c r="BC158" s="37"/>
     </row>
-    <row r="159" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:55" s="31" customFormat="1">
       <c r="A159" s="28" t="s">
         <v>682</v>
       </c>
@@ -30942,7 +31304,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="160" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:55" s="31" customFormat="1">
       <c r="A160" s="28" t="s">
         <v>682</v>
       </c>
@@ -31109,7 +31471,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="161" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A161" s="28" t="s">
         <v>682</v>
       </c>
@@ -31276,7 +31638,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="162" spans="1:55" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:55" s="31" customFormat="1" ht="28.8">
       <c r="A162" s="28" t="s">
         <v>682</v>
       </c>
@@ -31443,41 +31805,41 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="163" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:55" s="13" customFormat="1">
       <c r="A163" s="27"/>
     </row>
-    <row r="164" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="165" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="167" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:55" s="13" customFormat="1"/>
+    <row r="165" spans="1:55" s="13" customFormat="1"/>
+    <row r="166" spans="1:55" s="13" customFormat="1"/>
+    <row r="167" spans="1:55" s="13" customFormat="1">
       <c r="D167" s="14"/>
     </row>
-    <row r="168" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="169" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="171" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="188" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="189" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="190" spans="5:55" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:55" s="13" customFormat="1"/>
+    <row r="169" spans="1:55" s="13" customFormat="1"/>
+    <row r="170" spans="1:55" s="13" customFormat="1"/>
+    <row r="171" spans="1:55" s="13" customFormat="1"/>
+    <row r="172" spans="1:55" s="13" customFormat="1"/>
+    <row r="173" spans="1:55" s="13" customFormat="1"/>
+    <row r="174" spans="1:55" s="13" customFormat="1"/>
+    <row r="175" spans="1:55" s="13" customFormat="1"/>
+    <row r="176" spans="1:55" s="13" customFormat="1"/>
+    <row r="177" spans="5:55" s="13" customFormat="1"/>
+    <row r="178" spans="5:55" s="13" customFormat="1"/>
+    <row r="179" spans="5:55" s="13" customFormat="1"/>
+    <row r="180" spans="5:55" s="13" customFormat="1"/>
+    <row r="181" spans="5:55" s="13" customFormat="1"/>
+    <row r="182" spans="5:55" s="13" customFormat="1"/>
+    <row r="183" spans="5:55" s="13" customFormat="1"/>
+    <row r="184" spans="5:55" s="13" customFormat="1"/>
+    <row r="185" spans="5:55" s="13" customFormat="1"/>
+    <row r="186" spans="5:55" s="13" customFormat="1"/>
+    <row r="187" spans="5:55" s="13" customFormat="1"/>
+    <row r="188" spans="5:55" s="13" customFormat="1"/>
+    <row r="189" spans="5:55" s="13" customFormat="1"/>
+    <row r="190" spans="5:55" s="13" customFormat="1">
       <c r="F190" s="16"/>
     </row>
-    <row r="191" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:55" s="2" customFormat="1">
       <c r="E191" s="3"/>
       <c r="F191" s="18"/>
       <c r="G191" s="15"/>
@@ -31488,7 +31850,7 @@
       <c r="BB191" s="13"/>
       <c r="BC191" s="13"/>
     </row>
-    <row r="192" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:55" s="2" customFormat="1">
       <c r="E192" s="3"/>
       <c r="F192" s="18"/>
       <c r="G192" s="15"/>
@@ -31499,7 +31861,7 @@
       <c r="BB192" s="13"/>
       <c r="BC192" s="13"/>
     </row>
-    <row r="193" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="5:55" s="2" customFormat="1">
       <c r="E193" s="3"/>
       <c r="F193" s="18"/>
       <c r="G193" s="15"/>
@@ -31510,7 +31872,7 @@
       <c r="BB193" s="13"/>
       <c r="BC193" s="13"/>
     </row>
-    <row r="194" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="5:55" s="2" customFormat="1">
       <c r="E194" s="3"/>
       <c r="F194" s="18"/>
       <c r="G194" s="15"/>
@@ -31521,7 +31883,7 @@
       <c r="BB194" s="13"/>
       <c r="BC194" s="13"/>
     </row>
-    <row r="195" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="5:55" s="2" customFormat="1">
       <c r="E195" s="3"/>
       <c r="F195" s="18"/>
       <c r="G195" s="15"/>
@@ -31532,7 +31894,7 @@
       <c r="BB195" s="13"/>
       <c r="BC195" s="13"/>
     </row>
-    <row r="196" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="5:55" s="2" customFormat="1">
       <c r="E196" s="3"/>
       <c r="F196" s="18"/>
       <c r="G196" s="15"/>
@@ -31543,7 +31905,7 @@
       <c r="BB196" s="13"/>
       <c r="BC196" s="13"/>
     </row>
-    <row r="197" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="5:55" s="2" customFormat="1">
       <c r="E197" s="3"/>
       <c r="F197" s="18"/>
       <c r="G197" s="15"/>
@@ -31554,7 +31916,7 @@
       <c r="BB197" s="13"/>
       <c r="BC197" s="13"/>
     </row>
-    <row r="198" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="5:55" s="2" customFormat="1">
       <c r="E198" s="3"/>
       <c r="F198" s="18"/>
       <c r="G198" s="15"/>
@@ -31565,7 +31927,7 @@
       <c r="BB198" s="13"/>
       <c r="BC198" s="13"/>
     </row>
-    <row r="199" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="5:55" s="2" customFormat="1">
       <c r="E199" s="3"/>
       <c r="F199" s="18"/>
       <c r="G199" s="15"/>
@@ -31576,7 +31938,7 @@
       <c r="BB199" s="13"/>
       <c r="BC199" s="13"/>
     </row>
-    <row r="200" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="5:55" s="2" customFormat="1">
       <c r="E200" s="3"/>
       <c r="F200" s="18"/>
       <c r="G200" s="15"/>
@@ -31587,7 +31949,7 @@
       <c r="BB200" s="13"/>
       <c r="BC200" s="13"/>
     </row>
-    <row r="201" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="5:55" s="2" customFormat="1">
       <c r="E201" s="3"/>
       <c r="F201" s="18"/>
       <c r="G201" s="15"/>
@@ -31598,7 +31960,7 @@
       <c r="BB201" s="13"/>
       <c r="BC201" s="13"/>
     </row>
-    <row r="202" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="5:55" s="2" customFormat="1">
       <c r="E202" s="3"/>
       <c r="F202" s="18"/>
       <c r="G202" s="15"/>
@@ -31609,7 +31971,7 @@
       <c r="BB202" s="13"/>
       <c r="BC202" s="13"/>
     </row>
-    <row r="203" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="5:55" s="2" customFormat="1">
       <c r="E203" s="3"/>
       <c r="F203" s="18"/>
       <c r="G203" s="15"/>
@@ -31620,7 +31982,7 @@
       <c r="BB203" s="13"/>
       <c r="BC203" s="13"/>
     </row>
-    <row r="204" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="5:55" s="2" customFormat="1">
       <c r="E204" s="3"/>
       <c r="F204" s="18"/>
       <c r="G204" s="15"/>
@@ -31631,7 +31993,7 @@
       <c r="BB204" s="13"/>
       <c r="BC204" s="13"/>
     </row>
-    <row r="205" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="5:55" s="2" customFormat="1">
       <c r="E205" s="3"/>
       <c r="F205" s="18"/>
       <c r="G205" s="15"/>
@@ -31642,7 +32004,7 @@
       <c r="BB205" s="13"/>
       <c r="BC205" s="13"/>
     </row>
-    <row r="206" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="5:55" s="2" customFormat="1">
       <c r="E206" s="3"/>
       <c r="F206" s="18"/>
       <c r="G206" s="15"/>
@@ -31653,7 +32015,7 @@
       <c r="BB206" s="13"/>
       <c r="BC206" s="13"/>
     </row>
-    <row r="207" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="5:55" s="2" customFormat="1">
       <c r="E207" s="3"/>
       <c r="F207" s="18"/>
       <c r="G207" s="15"/>
@@ -31664,7 +32026,7 @@
       <c r="BB207" s="13"/>
       <c r="BC207" s="13"/>
     </row>
-    <row r="208" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="5:55" s="2" customFormat="1">
       <c r="E208" s="3"/>
       <c r="F208" s="18"/>
       <c r="G208" s="15"/>
@@ -31675,7 +32037,7 @@
       <c r="BB208" s="13"/>
       <c r="BC208" s="13"/>
     </row>
-    <row r="209" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="5:55" s="2" customFormat="1">
       <c r="E209" s="3"/>
       <c r="F209" s="11"/>
       <c r="G209" s="15"/>
@@ -31686,7 +32048,7 @@
       <c r="BB209" s="13"/>
       <c r="BC209" s="13"/>
     </row>
-    <row r="210" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="5:55" s="2" customFormat="1">
       <c r="E210" s="3"/>
       <c r="F210" s="18"/>
       <c r="G210" s="15"/>
@@ -31697,7 +32059,7 @@
       <c r="BB210" s="13"/>
       <c r="BC210" s="13"/>
     </row>
-    <row r="211" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="5:55" s="2" customFormat="1">
       <c r="E211" s="3"/>
       <c r="F211" s="18"/>
       <c r="G211" s="15"/>
@@ -31708,7 +32070,7 @@
       <c r="BB211" s="13"/>
       <c r="BC211" s="13"/>
     </row>
-    <row r="212" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="5:55" s="2" customFormat="1">
       <c r="E212" s="3"/>
       <c r="F212" s="18"/>
       <c r="G212" s="15"/>
@@ -31719,7 +32081,7 @@
       <c r="BB212" s="13"/>
       <c r="BC212" s="13"/>
     </row>
-    <row r="213" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="5:55" s="2" customFormat="1">
       <c r="E213" s="3"/>
       <c r="F213" s="18"/>
       <c r="G213" s="15"/>
@@ -31730,7 +32092,7 @@
       <c r="BB213" s="13"/>
       <c r="BC213" s="13"/>
     </row>
-    <row r="214" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="5:55" s="2" customFormat="1">
       <c r="E214" s="3"/>
       <c r="F214" s="18"/>
       <c r="G214" s="15"/>
@@ -31741,7 +32103,7 @@
       <c r="BB214" s="13"/>
       <c r="BC214" s="13"/>
     </row>
-    <row r="215" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="5:55" s="2" customFormat="1">
       <c r="E215" s="3"/>
       <c r="F215" s="18"/>
       <c r="G215" s="15"/>
@@ -31752,7 +32114,7 @@
       <c r="BB215" s="13"/>
       <c r="BC215" s="13"/>
     </row>
-    <row r="216" spans="5:55" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="5:55" s="2" customFormat="1">
       <c r="E216" s="3"/>
       <c r="F216" s="18"/>
       <c r="G216" s="15"/>
@@ -31763,11 +32125,11 @@
       <c r="BB216" s="13"/>
       <c r="BC216" s="13"/>
     </row>
-    <row r="217" spans="5:55" x14ac:dyDescent="0.3">
+    <row r="217" spans="5:55">
       <c r="F217" s="17"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A191:BC216">
+  <sortState ref="A191:BC216">
     <sortCondition ref="C191:C216"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>